<commit_message>
random no overlapping reactions
</commit_message>
<xml_diff>
--- a/simulator/NN_correlation_matrix/Results/Saved Models/Outputs/Sample0/Negative/neg_reaction0.xlsx
+++ b/simulator/NN_correlation_matrix/Results/Saved Models/Outputs/Sample0/Negative/neg_reaction0.xlsx
@@ -346,7 +346,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:BD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,40 +356,40 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J1" t="n">
         <v>12</v>
       </c>
       <c r="K1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M1" t="n">
         <v>16</v>
@@ -398,10 +398,130 @@
         <v>17</v>
       </c>
       <c r="O1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P1" t="n">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>21</v>
+      </c>
+      <c r="R1" t="n">
+        <v>22</v>
+      </c>
+      <c r="S1" t="n">
+        <v>23</v>
+      </c>
+      <c r="T1" t="n">
+        <v>24</v>
+      </c>
+      <c r="U1" t="n">
+        <v>25</v>
+      </c>
+      <c r="V1" t="n">
+        <v>27</v>
+      </c>
+      <c r="W1" t="n">
+        <v>29</v>
+      </c>
+      <c r="X1" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y1" t="n">
+        <v>32</v>
+      </c>
+      <c r="Z1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA1" t="n">
+        <v>35</v>
+      </c>
+      <c r="AB1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AD1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AE1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AF1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AG1" t="n">
+        <v>42</v>
+      </c>
+      <c r="AH1" t="n">
+        <v>46</v>
+      </c>
+      <c r="AI1" t="n">
+        <v>47</v>
+      </c>
+      <c r="AJ1" t="n">
+        <v>48</v>
+      </c>
+      <c r="AK1" t="n">
+        <v>49</v>
+      </c>
+      <c r="AL1" t="n">
+        <v>50</v>
+      </c>
+      <c r="AM1" t="n">
+        <v>51</v>
+      </c>
+      <c r="AN1" t="n">
+        <v>52</v>
+      </c>
+      <c r="AO1" t="n">
+        <v>53</v>
+      </c>
+      <c r="AP1" t="n">
+        <v>54</v>
+      </c>
+      <c r="AQ1" t="n">
+        <v>55</v>
+      </c>
+      <c r="AR1" t="n">
+        <v>58</v>
+      </c>
+      <c r="AS1" t="n">
+        <v>59</v>
+      </c>
+      <c r="AT1" t="n">
+        <v>60</v>
+      </c>
+      <c r="AU1" t="n">
+        <v>61</v>
+      </c>
+      <c r="AV1" t="n">
+        <v>63</v>
+      </c>
+      <c r="AW1" t="n">
+        <v>64</v>
+      </c>
+      <c r="AX1" t="n">
+        <v>65</v>
+      </c>
+      <c r="AY1" t="n">
+        <v>69</v>
+      </c>
+      <c r="AZ1" t="n">
+        <v>70</v>
+      </c>
+      <c r="BA1" t="n">
+        <v>72</v>
+      </c>
+      <c r="BB1" t="n">
+        <v>73</v>
+      </c>
+      <c r="BC1" t="n">
+        <v>74</v>
+      </c>
+      <c r="BD1" t="n">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>